<commit_message>
fixed initial conditions file RN SN problems, changed length-weight relationships in biol file
</commit_message>
<xml_diff>
--- a/R/length_weight_v15.xlsx
+++ b/R/length_weight_v15.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="length_weight_v15_data" sheetId="3" r:id="rId1"/>
@@ -2521,9 +2521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U591"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q4" sqref="Q4"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40965,7 +40965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS591"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E368" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>